<commit_message>
Update and run discrete data
</commit_message>
<xml_diff>
--- a/Results/german-credit-disc_results.xlsx
+++ b/Results/german-credit-disc_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,22 +459,70 @@
           <t>NCC robust</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>C4.5 acc</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>credal-C4.5 acc</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>SPN acc</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>CSPN low</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CSPN high</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>CSPN robust</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>69.85555555555555</v>
+        <v>69.88888888888889</v>
       </c>
       <c r="C2" t="n">
-        <v>69.43333333333334</v>
+        <v>69.44444444444444</v>
       </c>
       <c r="D2" t="n">
-        <v>70.3</v>
+        <v>70.31111111111112</v>
       </c>
       <c r="E2" t="n">
-        <v>70.04065652550436</v>
+        <v>70.05007533305347</v>
+      </c>
+      <c r="F2" t="n">
+        <v>64.82222222222222</v>
+      </c>
+      <c r="G2" t="n">
+        <v>65.03333333333333</v>
+      </c>
+      <c r="H2" t="n">
+        <v>69.67777777777778</v>
+      </c>
+      <c r="I2" t="n">
+        <v>69.67777777777778</v>
+      </c>
+      <c r="J2" t="n">
+        <v>69.67777777777778</v>
+      </c>
+      <c r="K2" t="n">
+        <v>69.67777777777778</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +530,34 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>71.07777777777778</v>
+        <v>70.52222222222223</v>
       </c>
       <c r="C3" t="n">
-        <v>70.53333333333333</v>
+        <v>70.12222222222222</v>
       </c>
       <c r="D3" t="n">
-        <v>71.56666666666666</v>
+        <v>70.84444444444445</v>
       </c>
       <c r="E3" t="n">
-        <v>71.26646473135111</v>
+        <v>70.63313254428461</v>
+      </c>
+      <c r="F3" t="n">
+        <v>58.01111111111111</v>
+      </c>
+      <c r="G3" t="n">
+        <v>59.68888888888888</v>
+      </c>
+      <c r="H3" t="n">
+        <v>70.04444444444445</v>
+      </c>
+      <c r="I3" t="n">
+        <v>56.33333333333334</v>
+      </c>
+      <c r="J3" t="n">
+        <v>79.14444444444445</v>
+      </c>
+      <c r="K3" t="n">
+        <v>73.18615626658946</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +565,34 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>70.01111111111112</v>
+        <v>70.83333333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>69.55555555555557</v>
+        <v>70.31111111111112</v>
       </c>
       <c r="D4" t="n">
-        <v>70.34444444444445</v>
+        <v>71.44444444444444</v>
       </c>
       <c r="E4" t="n">
-        <v>70.10949291685763</v>
+        <v>71.11849361731574</v>
+      </c>
+      <c r="F4" t="n">
+        <v>51.17777777777778</v>
+      </c>
+      <c r="G4" t="n">
+        <v>58.37777777777777</v>
+      </c>
+      <c r="H4" t="n">
+        <v>70.47777777777779</v>
+      </c>
+      <c r="I4" t="n">
+        <v>37.47777777777777</v>
+      </c>
+      <c r="J4" t="n">
+        <v>89.16666666666667</v>
+      </c>
+      <c r="K4" t="n">
+        <v>77.9314636777633</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +600,34 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>69.97777777777779</v>
+        <v>70.14444444444445</v>
       </c>
       <c r="C5" t="n">
-        <v>69.36666666666666</v>
+        <v>69.46666666666667</v>
       </c>
       <c r="D5" t="n">
-        <v>70.48888888888888</v>
+        <v>70.78888888888888</v>
       </c>
       <c r="E5" t="n">
-        <v>70.15259852192318</v>
+        <v>70.41087747269458</v>
+      </c>
+      <c r="F5" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>44.63333333333333</v>
+      </c>
+      <c r="H5" t="n">
+        <v>72.2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>25.28888888888889</v>
+      </c>
+      <c r="J5" t="n">
+        <v>91.75555555555555</v>
+      </c>
+      <c r="K5" t="n">
+        <v>74.90104613419182</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +635,34 @@
         <v>30</v>
       </c>
       <c r="B6" t="n">
-        <v>69.65555555555555</v>
+        <v>70.07777777777778</v>
       </c>
       <c r="C6" t="n">
-        <v>68.98888888888888</v>
+        <v>69.37777777777778</v>
       </c>
       <c r="D6" t="n">
-        <v>70.36666666666666</v>
+        <v>70.8</v>
       </c>
       <c r="E6" t="n">
-        <v>69.94984504501937</v>
+        <v>70.38341182815928</v>
+      </c>
+      <c r="F6" t="n">
+        <v>35.67777777777778</v>
+      </c>
+      <c r="G6" t="n">
+        <v>44.36666666666667</v>
+      </c>
+      <c r="H6" t="n">
+        <v>72.90000000000001</v>
+      </c>
+      <c r="I6" t="n">
+        <v>28.93333333333333</v>
+      </c>
+      <c r="J6" t="n">
+        <v>88.88888888888889</v>
+      </c>
+      <c r="K6" t="n">
+        <v>71.57912578987536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>